<commit_message>
name change as per dlrueda
</commit_message>
<xml_diff>
--- a/lane-locations.xlsx
+++ b/lane-locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmax/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B577AEE-EB8C-244A-8AB5-870E37D90724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6383CC57-2C66-2443-A6AB-13275CF9F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,13 +53,13 @@
     <t>LANE-ACQ</t>
   </si>
   <si>
-    <t>Lane -- Acquisitions</t>
+    <t>Lane  Acquisitions</t>
   </si>
   <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>Lane -- ACQ</t>
+    <t>Lane ACQ</t>
   </si>
   <si>
     <t>SU</t>
@@ -77,1216 +77,1216 @@
     <t>LANE-APER</t>
   </si>
   <si>
-    <t>Lane -- Offsite: Periodicals*</t>
-  </si>
-  <si>
-    <t>Lane -- Offsite:  Periodicals* (Click on \"Requests\")</t>
+    <t>Lane Offsite: Periodicals*</t>
+  </si>
+  <si>
+    <t>Lane Offsite:  Periodicals* (Click on \"Requests\")</t>
   </si>
   <si>
     <t>LANE-ARAB</t>
   </si>
   <si>
-    <t>Lane -- Spec: Arabic</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Arabic: By appointment only.</t>
+    <t>Lane Spec: Arabic</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Arabic: By appointment only.</t>
   </si>
   <si>
     <t>LANE-ARASZ</t>
   </si>
   <si>
-    <t>Lane -- Spec: Arabic Oversize</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Arabic Oversize: By appointment only.</t>
+    <t>Lane Spec: Arabic Oversize</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Arabic Oversize: By appointment only.</t>
   </si>
   <si>
     <t>LANE-ARCH</t>
   </si>
   <si>
-    <t>Lane -- Spec: Archives Class</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Archives Class.: By appointment only.</t>
+    <t>Lane Spec: Archives Class</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Archives Class.: By appointment only.</t>
   </si>
   <si>
     <t>LANE-AV</t>
   </si>
   <si>
-    <t>Lane -- Media: AV</t>
-  </si>
-  <si>
-    <t>Lane -- Media: AV (Compact Shelving next to History)</t>
+    <t>Lane Media: AV</t>
+  </si>
+  <si>
+    <t>Lane Media: AV (Compact Shelving next to History)</t>
   </si>
   <si>
     <t>LANE-BOOK</t>
   </si>
   <si>
-    <t>Lane -- Media: Books</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Books (FLRC Upstairs)</t>
+    <t>Lane Media: Books</t>
+  </si>
+  <si>
+    <t>Lane Media: Books (FLRC Upstairs)</t>
   </si>
   <si>
     <t>LANE-BSP</t>
   </si>
   <si>
-    <t>Lane -- Bound/Shelved w/Parent</t>
-  </si>
-  <si>
-    <t>Lane -- Click Parent: link for access options</t>
+    <t>Lane Bound/Shelved w/Parent</t>
+  </si>
+  <si>
+    <t>Lane Click Parent: link for access options</t>
   </si>
   <si>
     <t>LANE-BSW</t>
   </si>
   <si>
-    <t>Lane -- Bound/Shelved Elsewhere</t>
-  </si>
-  <si>
-    <t>Lane -- Click Related: link for access options</t>
+    <t>Lane Bound/Shelved Elsewhere</t>
+  </si>
+  <si>
+    <t>Lane Click Related: link for access options</t>
   </si>
   <si>
     <t>LANE-CAT</t>
   </si>
   <si>
-    <t>Lane -- Bibliographic  Mgmt</t>
-  </si>
-  <si>
-    <t>Lane -- CAT</t>
+    <t>Lane  Bibliographic  Mgmt</t>
+  </si>
+  <si>
+    <t>Lane CAT</t>
   </si>
   <si>
     <t>LANE-CDLC</t>
   </si>
   <si>
-    <t>Lane -- Books: LC Class CDs</t>
-  </si>
-  <si>
-    <t>Lane -- Books: LC Class CD Collection (Shelved at User Services Desk</t>
+    <t>Lane Books: LC Class CDs</t>
+  </si>
+  <si>
+    <t>Lane Books: LC Class CD Collection (Shelved at User Services Desk</t>
   </si>
   <si>
     <t>LANE-CDPER</t>
   </si>
   <si>
-    <t>Lane -- CD Periodicals</t>
-  </si>
-  <si>
-    <t>Lane -- .Periodicals:  CDs Shelved by Title</t>
+    <t>Lane CD Periodicals</t>
+  </si>
+  <si>
+    <t>Lane .Periodicals:  CDs Shelved by Title</t>
   </si>
   <si>
     <t>LANE-CIRC</t>
   </si>
   <si>
-    <t>Lane -- Circulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane -- </t>
+    <t>Lane  Circulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane </t>
   </si>
   <si>
     <t>LANE-COM</t>
   </si>
   <si>
-    <t>Lane -- Per: Compact</t>
-  </si>
-  <si>
-    <t>Lane -- .Periodicals (holding area)</t>
+    <t>Lane Per: Compact</t>
+  </si>
+  <si>
+    <t>Lane .Periodicals (holding area)</t>
   </si>
   <si>
     <t>LANE-COMP</t>
   </si>
   <si>
-    <t>Lane -- Component</t>
-  </si>
-  <si>
-    <t>Lane -- Click Component of: link(s) for access options</t>
+    <t>Lane Component</t>
+  </si>
+  <si>
+    <t>Lane Click Component of: link(s) for access options</t>
   </si>
   <si>
     <t>LANE-COR</t>
   </si>
   <si>
-    <t>Lane -- Per: Core</t>
-  </si>
-  <si>
-    <t>Lane -- .Periodicals: A-Z</t>
+    <t>Lane Per: Core</t>
+  </si>
+  <si>
+    <t>Lane .Periodicals: A-Z</t>
   </si>
   <si>
     <t>LANE-CRDSK</t>
   </si>
   <si>
-    <t>Lane -- Circ Desk Collection</t>
-  </si>
-  <si>
-    <t>Lane -- Audio CDs: Shelved at User Services Desk</t>
+    <t>Lane Circ Desk Collection</t>
+  </si>
+  <si>
+    <t>Lane Audio CDs: Shelved at User Services Desk</t>
   </si>
   <si>
     <t>LANE-CRES</t>
   </si>
   <si>
-    <t>Lane -- Course Reserves</t>
-  </si>
-  <si>
-    <t>Lane -- Reserves: Course Reserves</t>
+    <t>Lane Course Reserves</t>
+  </si>
+  <si>
+    <t>Lane Reserves: Course Reserves</t>
   </si>
   <si>
     <t>LANE-DCORE</t>
   </si>
   <si>
-    <t>Lane -- Books: DCORE</t>
-  </si>
-  <si>
-    <t>Lane -- Books: DCORE (Downstairs DCORE)</t>
+    <t>Lane Books: DCORE</t>
+  </si>
+  <si>
+    <t>Lane Books: DCORE (Downstairs DCORE)</t>
   </si>
   <si>
     <t>LANE-DESKCOPY</t>
   </si>
   <si>
-    <t>Lane -- Staff:  Desk Copy</t>
+    <t>Lane Staff:  Desk Copy</t>
   </si>
   <si>
     <t>LANE-DTBS</t>
   </si>
   <si>
-    <t>Lane -- Digital: Database</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Database</t>
+    <t>Lane Digital: Database</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Database</t>
   </si>
   <si>
     <t>LANE-ECOLL</t>
   </si>
   <si>
-    <t>Lane -- Digital: Collection</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Collection</t>
+    <t>Lane Digital: Collection</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Collection</t>
   </si>
   <si>
     <t>LANE-ECOMP</t>
   </si>
   <si>
-    <t>Lane -- Digital Component</t>
-  </si>
-  <si>
-    <t>Lane -- Click Full Text @ Lane Library Stanford button for access</t>
+    <t>Lane Digital Component</t>
+  </si>
+  <si>
+    <t>Lane Click Full Text @ Lane Library Stanford button for access</t>
   </si>
   <si>
     <t>LANE-EDATA</t>
   </si>
   <si>
-    <t>Lane -- Digital: Access</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Access</t>
+    <t>Lane Digital: Access</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Access</t>
   </si>
   <si>
     <t>LANE-EDOC</t>
   </si>
   <si>
-    <t>Lane -- Digital: Document</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Document</t>
+    <t>Lane Digital: Document</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Document</t>
   </si>
   <si>
     <t>LANE-EFEE</t>
   </si>
   <si>
-    <t>Lane -- Digital: Fee for Access</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Fee for Access</t>
+    <t>Lane Digital: Fee for Access</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Fee for Access</t>
   </si>
   <si>
     <t>LANE-EPER</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 0</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Periodical</t>
+    <t>Lane Digital: Periodical 0</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Periodical</t>
   </si>
   <si>
     <t>LANE-EPER1</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 1</t>
+    <t>Lane Digital: Periodical 1</t>
   </si>
   <si>
     <t>LANE-EPER2</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 2</t>
+    <t>Lane Digital: Periodical 2</t>
   </si>
   <si>
     <t>LANE-EPER3</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 3</t>
+    <t>Lane Digital: Periodical 3</t>
   </si>
   <si>
     <t>LANE-EPER4</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 4</t>
+    <t>Lane Digital: Periodical 4</t>
   </si>
   <si>
     <t>LANE-EPER5</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 5</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Periodical (Metered Access)</t>
+    <t>Lane Digital: Periodical 5</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Periodical (Metered Access)</t>
   </si>
   <si>
     <t>LANE-EPER6</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 6</t>
+    <t>Lane Digital: Periodical 6</t>
   </si>
   <si>
     <t>LANE-EPER7</t>
   </si>
   <si>
-    <t>Lane -- Digital: Periodical 7</t>
+    <t>Lane Digital: Periodical 7</t>
   </si>
   <si>
     <t>LANE-EQUIP</t>
   </si>
   <si>
-    <t>Lane -- Equipment</t>
+    <t>Lane  Equipment</t>
   </si>
   <si>
     <t>LANE-ERQC</t>
   </si>
   <si>
-    <t>Lane -- Exam Reviews</t>
-  </si>
-  <si>
-    <t>Lane -- Reserves: Exam Review Books (shelved at User Services Desk)</t>
+    <t>Lane Exam Reviews</t>
+  </si>
+  <si>
+    <t>Lane Reserves: Exam Review Books (shelved at User Services Desk)</t>
   </si>
   <si>
     <t>LANE-FLAT</t>
   </si>
   <si>
-    <t>Lane -- Books: Oversize Flat</t>
-  </si>
-  <si>
-    <t>Lane -- Books: Oversize - Flat (Downstairs)</t>
+    <t>Lane Books: Oversize Flat</t>
+  </si>
+  <si>
+    <t>Lane Books: Oversize - Flat (Downstairs)</t>
   </si>
   <si>
     <t>LANE-FOLIO</t>
   </si>
   <si>
-    <t>Lane -- Books: Oversize Folio</t>
-  </si>
-  <si>
-    <t>Lane -- Books: Oversize - Folio (Downstairs)</t>
+    <t>Lane Books: Oversize Folio</t>
+  </si>
+  <si>
+    <t>Lane Books: Oversize - Folio (Downstairs)</t>
   </si>
   <si>
     <t>LANE-FOLIO.</t>
   </si>
   <si>
-    <t>Lane -- Books: Oversize FOLIO.</t>
+    <t>Lane Books: Oversize FOLIO.</t>
   </si>
   <si>
     <t>LANE-FOTOF</t>
   </si>
   <si>
-    <t>Lane -- Spec: Photofile</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Photo File: By appointment only.</t>
+    <t>Lane Spec: Photofile</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Photo File: By appointment only.</t>
   </si>
   <si>
     <t>LANE-FPER</t>
   </si>
   <si>
-    <t>Lane -- Media: Periodicals</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Compact Shelves (Downstairs)</t>
+    <t>Lane Media: Periodicals</t>
+  </si>
+  <si>
+    <t>Lane Media: Compact Shelves (Downstairs)</t>
   </si>
   <si>
     <t>LANE-FSDOC</t>
   </si>
   <si>
-    <t>Lane -- Media: Documentation</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Documentation (FLRC Upstairs)</t>
+    <t>Lane Media: Documentation</t>
+  </si>
+  <si>
+    <t>Lane Media: Documentation (FLRC Upstairs)</t>
   </si>
   <si>
     <t>LANE-FSOFT</t>
   </si>
   <si>
-    <t>Lane -- Media: Software</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Software (FLRC Upstairs)</t>
+    <t>Lane Media: Software</t>
+  </si>
+  <si>
+    <t>Lane Media: Software (FLRC Upstairs)</t>
   </si>
   <si>
     <t>LANE-FTHSS</t>
   </si>
   <si>
-    <t>Lane -- Offsite: Theses</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Theses (Click on \"Request\" Link Above)</t>
+    <t>Lane Offsite: Theses</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Theses (Click on \"Request\" Link Above)</t>
   </si>
   <si>
     <t>LANE-GRATS</t>
   </si>
   <si>
-    <t>Lane -- Staff: Free</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Free Material</t>
+    <t>Lane Staff: Free</t>
+  </si>
+  <si>
+    <t>Lane Staff: Free Material</t>
   </si>
   <si>
     <t>LANE-HIST</t>
   </si>
   <si>
-    <t>Lane -- Books: History - LC</t>
-  </si>
-  <si>
-    <t>Lane -- Books: History - LC Classification (Downstairs)</t>
+    <t>Lane Books: History - LC</t>
+  </si>
+  <si>
+    <t>Lane Books: History - LC Classification (Downstairs)</t>
   </si>
   <si>
     <t>LANE-HSFLE</t>
   </si>
   <si>
-    <t>Lane -- Spec: Vertical File</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Vertical File: By appointment only.</t>
+    <t>Lane Spec: Vertical File</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Vertical File: By appointment only.</t>
   </si>
   <si>
     <t>LANE-IFOAV</t>
   </si>
   <si>
-    <t>Lane -- Instr: Materials</t>
-  </si>
-  <si>
-    <t>Lane -- Instructional: Materials</t>
+    <t>Lane Instr: Materials</t>
+  </si>
+  <si>
+    <t>Lane Instructional: Materials</t>
   </si>
   <si>
     <t>LANE-IFOEQ</t>
   </si>
   <si>
-    <t>Lane -- Instr: Equipment</t>
-  </si>
-  <si>
-    <t>Lane -- Instructional: Equipment</t>
+    <t>Lane Instr: Equipment</t>
+  </si>
+  <si>
+    <t>Lane Instructional: Equipment</t>
   </si>
   <si>
     <t>LANE-ILLDK</t>
   </si>
   <si>
-    <t>Lane -- Staff: ILL</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Interlibrary Loan</t>
+    <t>Lane Staff: ILL</t>
+  </si>
+  <si>
+    <t>Lane Staff: Interlibrary Loan</t>
   </si>
   <si>
     <t>LANE-IMAGE</t>
   </si>
   <si>
-    <t>Lane -- Digital: Image</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Image</t>
+    <t>Lane Digital: Image</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Image</t>
   </si>
   <si>
     <t>LANE-IMMI</t>
   </si>
   <si>
-    <t>Lane -- Not Owned: IMMI</t>
-  </si>
-  <si>
-    <t>Lane -- Not Owned: Index to Medieval Medical Images</t>
+    <t>Lane Not Owned: IMMI</t>
+  </si>
+  <si>
+    <t>Lane Not Owned: Index to Medieval Medical Images</t>
   </si>
   <si>
     <t>LANE-INCAT</t>
   </si>
   <si>
-    <t>Lane -- Spec: Instrument Catalogs</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Instrument Catalogs-By appointment only</t>
+    <t>Lane Spec: Instrument Catalogs</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Instrument Catalogs-By appointment only</t>
   </si>
   <si>
     <t>LANE-INDEX</t>
   </si>
   <si>
-    <t>Lane -- Ref: Computer Tables</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Computer Tables</t>
+    <t>Lane Ref: Computer Tables</t>
+  </si>
+  <si>
+    <t>Lane Reference: Computer Tables</t>
   </si>
   <si>
     <t>LANE-INSTR</t>
   </si>
   <si>
-    <t>Lane -- Spec: Instruments</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Instruments (Stored offsite)</t>
+    <t>Lane Spec: Instruments</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Instruments (Stored offsite)</t>
   </si>
   <si>
     <t>LANE-ISIIF</t>
   </si>
   <si>
-    <t>Lane -- Digital: Impact Factor</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Impact Factor</t>
+    <t>Lane Digital: Impact Factor</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Impact Factor</t>
   </si>
   <si>
     <t>LANE-LAN</t>
   </si>
   <si>
-    <t>Lane -- Books: LC Class</t>
-  </si>
-  <si>
-    <t>Lane -- Books: General Collection (Downstairs)</t>
+    <t>Lane Books: LC Class</t>
+  </si>
+  <si>
+    <t>Lane Books: General Collection (Downstairs)</t>
   </si>
   <si>
     <t>LANE-LASER</t>
   </si>
   <si>
-    <t>Lane -- Media: Laser Disks</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Laser Disks (Downstairs behind Elevator)</t>
+    <t>Lane Media: Laser Disks</t>
+  </si>
+  <si>
+    <t>Lane Media: Laser Disks (Downstairs behind Elevator)</t>
   </si>
   <si>
     <t>LANE-LC2</t>
   </si>
   <si>
-    <t>Lane -- Offsite: LC Class 2</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: LC Classification 2</t>
+    <t>Lane Offsite: LC Class 2</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: LC Classification 2</t>
   </si>
   <si>
     <t>LANE-LECT</t>
   </si>
   <si>
-    <t>Lane -- Media: Video Lectures</t>
+    <t>Lane Media: Video Lectures</t>
   </si>
   <si>
     <t>LANE-LIBR</t>
   </si>
   <si>
-    <t>Lane -- Staff: Lib Lit</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Library Literature Collection</t>
+    <t>Lane Staff: Lib Lit</t>
+  </si>
+  <si>
+    <t>Lane Staff: Library Literature Collection</t>
   </si>
   <si>
     <t>LANE-LKSC</t>
   </si>
   <si>
-    <t>Lane -- Li Ka Shing Center</t>
+    <t>Lane Li Ka Shing Center</t>
   </si>
   <si>
     <t>LANE-MAP</t>
   </si>
   <si>
-    <t>Lane -- Spec: Map Case</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Map Case: By appointment only.</t>
+    <t>Lane Spec: Map Case</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Map Case: By appointment only.</t>
   </si>
   <si>
     <t>LANE-MICRO</t>
   </si>
   <si>
-    <t>Lane -- Ref: Microform Cabinet</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Microform Cabinet</t>
+    <t>Lane Ref: Microform Cabinet</t>
+  </si>
+  <si>
+    <t>Lane Reference: Microform Cabinet</t>
   </si>
   <si>
     <t>LANE-MINI</t>
   </si>
   <si>
-    <t>Lane -- Spec: Mini</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Miniature: By appointment only.</t>
+    <t>Lane Spec: Mini</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Miniature: By appointment only.</t>
   </si>
   <si>
     <t>LANE-MISC</t>
   </si>
   <si>
-    <t>Lane -- Books: Miscellaneous</t>
-  </si>
-  <si>
-    <t>Lane -- Books: See Holdings Note for Location</t>
+    <t>Lane Books: Miscellaneous</t>
+  </si>
+  <si>
+    <t>Lane Books: See Holdings Note for Location</t>
   </si>
   <si>
     <t>LANE-MOBI</t>
   </si>
   <si>
-    <t>Lane -- Digital: Mobile Resources</t>
-  </si>
-  <si>
-    <t>Lane -- .Digital: Mobile Resources</t>
+    <t>Lane Digital: Mobile Resources</t>
+  </si>
+  <si>
+    <t>Lane .Digital: Mobile Resources</t>
   </si>
   <si>
     <t>LANE-MODEL</t>
   </si>
   <si>
-    <t>Lane -- Media: Models</t>
+    <t>Lane Media: Models</t>
   </si>
   <si>
     <t>LANE-MSS</t>
   </si>
   <si>
-    <t>Lane -- Spec: Manuscipts</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Manuscripts: By appointment only.</t>
+    <t>Lane Spec: Manuscipts</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Manuscripts: By appointment only.</t>
   </si>
   <si>
     <t>LANE-NEWB</t>
   </si>
   <si>
-    <t>Lane -- New Books</t>
-  </si>
-  <si>
-    <t>Lane -- New Books Shelf</t>
+    <t>Lane New Books</t>
+  </si>
+  <si>
+    <t>Lane New Books Shelf</t>
   </si>
   <si>
     <t>LANE-NEWS</t>
   </si>
   <si>
-    <t>Lane -- Per: Newspapers</t>
-  </si>
-  <si>
-    <t>Lane -- .Periodicals: Newspapers</t>
+    <t>Lane Per: Newspapers</t>
+  </si>
+  <si>
+    <t>Lane .Periodicals: Newspapers</t>
   </si>
   <si>
     <t>LANE-NLOC</t>
   </si>
   <si>
-    <t>Lane -- Error: Loc Problem in Acq</t>
-  </si>
-  <si>
-    <t>Lane -- Error: Location Problem</t>
+    <t>Lane Error: Loc Problem in Acq</t>
+  </si>
+  <si>
+    <t>Lane Error: Location Problem</t>
   </si>
   <si>
     <t>LANE-NOLOC</t>
   </si>
   <si>
-    <t>Lane -- Error: Location Lacking</t>
-  </si>
-  <si>
-    <t>Lane -- Books: LC Classification or On Reserve</t>
+    <t>Lane Error: Location Lacking</t>
+  </si>
+  <si>
+    <t>Lane Books: LC Classification or On Reserve</t>
   </si>
   <si>
     <t>LANE-OHIST</t>
   </si>
   <si>
-    <t>Lane -- Books: History - Old Clas</t>
-  </si>
-  <si>
-    <t>Lane -- Books: History - Old Classification (Downstairs)</t>
+    <t>Lane Books: History - Old Clas</t>
+  </si>
+  <si>
+    <t>Lane Books: History - Old Classification (Downstairs)</t>
   </si>
   <si>
     <t>LANE-OLC</t>
   </si>
   <si>
-    <t>Lane -- Staff: Online Collection</t>
+    <t>Lane Staff: Online Collection</t>
   </si>
   <si>
     <t>LANE-OLD</t>
   </si>
   <si>
-    <t>Lane -- Offsit: OldClass1925-1976</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Old Class (1925-1976) Click on \"Request\" Link Above</t>
+    <t>Lane Offsit: OldClass1925-1976</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Old Class (1925-1976) Click on \"Request\" Link Above</t>
   </si>
   <si>
     <t>LANE-OVPER</t>
   </si>
   <si>
-    <t>Lane -- Per: Oversize</t>
-  </si>
-  <si>
-    <t>Lane -- .Periodicals: Oversize (Compact Shelves Downstairs)</t>
+    <t>Lane Per: Oversize</t>
+  </si>
+  <si>
+    <t>Lane .Periodicals: Oversize (Compact Shelves Downstairs)</t>
   </si>
   <si>
     <t>LANE-OVSZE</t>
   </si>
   <si>
-    <t>Lane -- Books: Oversize</t>
-  </si>
-  <si>
-    <t>Lane -- Books: Oversize (Downstairs)</t>
+    <t>Lane Books: Oversize</t>
+  </si>
+  <si>
+    <t>Lane Books: Oversize (Downstairs)</t>
   </si>
   <si>
     <t>LANE-PANL</t>
   </si>
   <si>
-    <t>Lane -- Print Analytic</t>
-  </si>
-  <si>
-    <t>Lane -- Click on Series link(s) for access options</t>
+    <t>Lane Print Analytic</t>
+  </si>
+  <si>
+    <t>Lane Click on Series link(s) for access options</t>
   </si>
   <si>
     <t>LANE-PARCH</t>
   </si>
   <si>
-    <t>Lane -- Spec: Per Archives</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections:Archival Periodicals:By appointment only</t>
+    <t>Lane Spec: Per Archives</t>
+  </si>
+  <si>
+    <t>Lane Special Collections:Archival Periodicals:By appointment only</t>
   </si>
   <si>
     <t>LANE-PAV</t>
   </si>
   <si>
-    <t>Lane -- Media: Audiocassettes</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Audio CDs (Duck Room)</t>
+    <t>Lane Media: Audiocassettes</t>
+  </si>
+  <si>
+    <t>Lane Media: Audio CDs (Duck Room)</t>
   </si>
   <si>
     <t>LANE-PCOMP</t>
   </si>
   <si>
-    <t>Lane -- Print Component</t>
-  </si>
-  <si>
-    <t>Lane -- Click 'Component of:' title(s) or Stanford button for access</t>
+    <t>Lane Print Component</t>
+  </si>
+  <si>
+    <t>Lane Click 'Component of:' title(s) or Stanford button for access</t>
   </si>
   <si>
     <t>LANE-PER</t>
   </si>
   <si>
-    <t>Lane -- Per: A-Z</t>
+    <t>Lane Per: A-Z</t>
   </si>
   <si>
     <t>LANE-PLIBR</t>
   </si>
   <si>
-    <t>Lane -- Staff: Lib Lit Periodical</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Library Literature Periodicals</t>
+    <t>Lane Staff: Lib Lit Periodical</t>
+  </si>
+  <si>
+    <t>Lane Staff: Library Literature Periodicals</t>
   </si>
   <si>
     <t>LANE-PMICR</t>
   </si>
   <si>
-    <t>Lane -- Ref: Microform Per</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Microform Periodicals</t>
+    <t>Lane Ref: Microform Per</t>
+  </si>
+  <si>
+    <t>Lane Reference: Microform Periodicals</t>
   </si>
   <si>
     <t>LANE-POLC</t>
   </si>
   <si>
-    <t>Lane -- Staff: Online Coll Per</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Online Collection Periodicals</t>
+    <t>Lane Staff: Online Coll Per</t>
+  </si>
+  <si>
+    <t>Lane Staff: Online Collection Periodicals</t>
   </si>
   <si>
     <t>LANE-PORT</t>
   </si>
   <si>
-    <t>Lane -- Spec: Portraits (Annex)</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Portraits (Annex): By appointment only.</t>
+    <t>Lane Spec: Portraits (Annex)</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Portraits (Annex): By appointment only.</t>
   </si>
   <si>
     <t>LANE-PREF</t>
   </si>
   <si>
-    <t>Lane -- Ref: Periodicals</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Periodicals</t>
+    <t>Lane Ref: Periodicals</t>
+  </si>
+  <si>
+    <t>Lane Reference: Periodicals</t>
   </si>
   <si>
     <t>LANE-PRES</t>
   </si>
   <si>
-    <t>Lane -- Personal Copy</t>
+    <t>Lane Personal Copy</t>
   </si>
   <si>
     <t>LANE-PROLC</t>
   </si>
   <si>
-    <t>Lane -- Staff: Online Retired</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Online Collection - Retired</t>
+    <t>Lane Staff: Online Retired</t>
+  </si>
+  <si>
+    <t>Lane Staff: Online Collection - Retired</t>
   </si>
   <si>
     <t>LANE-PRREF</t>
   </si>
   <si>
-    <t>Lane -- Ref: Retired Periodical</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Periodicals - Retired(Compact Shelves Downstairs)</t>
+    <t>Lane Ref: Retired Periodical</t>
+  </si>
+  <si>
+    <t>Lane Reference: Periodicals - Retired(Compact Shelves Downstairs)</t>
   </si>
   <si>
     <t>LANE-PRSV</t>
   </si>
   <si>
-    <t>Lane -- Reserve Periodical</t>
-  </si>
-  <si>
-    <t>Lane -- Reserves: Periodicals</t>
+    <t>Lane Reserve Periodical</t>
+  </si>
+  <si>
+    <t>Lane Reserves: Periodicals</t>
   </si>
   <si>
     <t>LANE-PSPEC</t>
   </si>
   <si>
-    <t>Lane -- Spec: Periodicals</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Rare Periodicals: By appointment only.</t>
+    <t>Lane Spec: Periodicals</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Rare Periodicals: By appointment only.</t>
   </si>
   <si>
     <t>LANE-PTS</t>
   </si>
   <si>
-    <t>Lane -- Staff: RM Per</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Resource Management - Periodicals</t>
+    <t>Lane Staff: RM Per</t>
+  </si>
+  <si>
+    <t>Lane Staff: Resource Management - Periodicals</t>
   </si>
   <si>
     <t>LANE-QUERY</t>
   </si>
   <si>
-    <t>Lane -- Not Owned: Request Loan</t>
-  </si>
-  <si>
-    <t>Lane -- Not Owned: Request Interlibrary Loan</t>
+    <t>Lane Not Owned: Request Loan</t>
+  </si>
+  <si>
+    <t>Lane Not Owned: Request Interlibrary Loan</t>
   </si>
   <si>
     <t>LANE-REF</t>
   </si>
   <si>
-    <t>Lane -- Ref: LC Class</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: LC Classification</t>
+    <t>Lane Ref: LC Class</t>
+  </si>
+  <si>
+    <t>Lane Reference: LC Classification</t>
   </si>
   <si>
     <t>LANE-REFREV</t>
   </si>
   <si>
-    <t>Lane -- Ref: Reference Review</t>
-  </si>
-  <si>
-    <t>Lane -- Ref: Reference Review Shelf</t>
+    <t>Lane Ref: Reference Review</t>
+  </si>
+  <si>
+    <t>Lane Ref: Reference Review Shelf</t>
   </si>
   <si>
     <t>LANE-RES</t>
   </si>
   <si>
-    <t>Lane -- Core Textbooks</t>
+    <t>Lane Core Textbooks</t>
   </si>
   <si>
     <t>LANE-REVIEW</t>
   </si>
   <si>
-    <t>Lane -- Error: REVIEW</t>
-  </si>
-  <si>
-    <t>Lane -- Error: Location Problem - Please Report</t>
+    <t>Lane Error: REVIEW</t>
+  </si>
+  <si>
+    <t>Lane Error: Location Problem - Please Report</t>
   </si>
   <si>
     <t>LANE-RFDSK</t>
   </si>
   <si>
-    <t>Lane -- Ref: Desk</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Ask at Desk</t>
+    <t>Lane Ref: Desk</t>
+  </si>
+  <si>
+    <t>Lane Reference: Ask at Desk</t>
   </si>
   <si>
     <t>LANE-RFFLE</t>
   </si>
   <si>
-    <t>Lane -- Ref: File</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: File Cabinet</t>
+    <t>Lane Ref: File</t>
+  </si>
+  <si>
+    <t>Lane Reference: File Cabinet</t>
   </si>
   <si>
     <t>LANE-RLIN</t>
   </si>
   <si>
-    <t>Lane -- Staff: RLIN Docs</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: RLIN Documentation</t>
+    <t>Lane Staff: RLIN Docs</t>
+  </si>
+  <si>
+    <t>Lane Staff: RLIN Documentation</t>
   </si>
   <si>
     <t>LANE-RLOC</t>
   </si>
   <si>
-    <t>Lane -- Ref: Ref or Retired Ref</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Ref or Retired Ref</t>
+    <t>Lane Ref: Ref or Retired Ref</t>
+  </si>
+  <si>
+    <t>Lane Reference: Ref or Retired Ref</t>
   </si>
   <si>
     <t>LANE-ROLC</t>
   </si>
   <si>
-    <t>Lane -- Ref: Retired Online</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Retired Online</t>
+    <t>Lane Ref: Retired Online</t>
+  </si>
+  <si>
+    <t>Lane Reference: Retired Online</t>
   </si>
   <si>
     <t>LANE-RREF</t>
   </si>
   <si>
-    <t>Lane -- Ref: Retired</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Retired LC Class (Downstairs)</t>
+    <t>Lane Ref: Retired</t>
+  </si>
+  <si>
+    <t>Lane Reference: Retired LC Class (Downstairs)</t>
   </si>
   <si>
     <t>LANE-RREF2</t>
   </si>
   <si>
-    <t>Lane -- Offsite: Retired Ref</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Retired Reference LC Class (Click on \"Request\" Link</t>
+    <t>Lane Offsite: Retired Ref</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Retired Reference LC Class (Click on \"Request\" Link</t>
   </si>
   <si>
     <t>LANE-RTHSS</t>
   </si>
   <si>
-    <t>Lane -- Spec: Theses</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Theses: By appointment only.</t>
+    <t>Lane Spec: Theses</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Theses: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SAL3</t>
   </si>
   <si>
-    <t>Lane -- Offsite:  SAL3</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Click on \"Request\" Link Above</t>
+    <t>Lane Offsite:  SAL3</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Click on \"Request\" Link Above</t>
   </si>
   <si>
     <t>LANE-SAL3X</t>
   </si>
   <si>
-    <t>Lane -- Offsite: Mediated</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Permission required; contact Service Desk</t>
+    <t>Lane Offsite: Mediated</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Permission required; contact Service Desk</t>
   </si>
   <si>
     <t>LANE-SC1</t>
   </si>
   <si>
-    <t>Lane -- Self Check SoMCC</t>
+    <t>Lane Self Check SoMCC</t>
   </si>
   <si>
     <t>LANE-SCAN</t>
   </si>
   <si>
-    <t>Lane -- Temp Unavailable</t>
-  </si>
-  <si>
-    <t>Lane -- Temporarily unavailable; request Interlibrary Loan.</t>
+    <t>Lane  Temp Unavailable</t>
+  </si>
+  <si>
+    <t>Lane Temporarily unavailable; request Interlibrary Loan.</t>
   </si>
   <si>
     <t>LANE-SDOC</t>
   </si>
   <si>
-    <t>Lane -- Staff: Software Doc</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Software Documentation</t>
+    <t>Lane Staff: Software Doc</t>
+  </si>
+  <si>
+    <t>Lane Staff: Software Documentation</t>
   </si>
   <si>
     <t>LANE-SELF</t>
   </si>
   <si>
-    <t>Lane -- Self Check</t>
+    <t>Lane Self Check</t>
   </si>
   <si>
     <t>LANE-SERIES</t>
   </si>
   <si>
-    <t>Lane -- Books: Rel Title Browse</t>
-  </si>
-  <si>
-    <t>Lane -- Varies.</t>
+    <t>Lane Books: Rel Title Browse</t>
+  </si>
+  <si>
+    <t>Lane Varies.</t>
   </si>
   <si>
     <t>LANE-SFLAT</t>
   </si>
   <si>
-    <t>Lane -- Spec: LC Oversize - Flat</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: LC Oversize-Flat: By appointment only.</t>
+    <t>Lane Spec: LC Oversize - Flat</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: LC Oversize-Flat: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SFOL</t>
   </si>
   <si>
-    <t>Lane -- Spec: LC Oversize - Folio</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: LC Oversize-Folio: By appointment only.</t>
+    <t>Lane Spec: LC Oversize - Folio</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: LC Oversize-Folio: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SIMUL</t>
   </si>
   <si>
-    <t>Lane -- Media: Simulations</t>
-  </si>
-  <si>
-    <t>Lane -- Media: Simulations (FLRC Upstairs)</t>
+    <t>Lane Media: Simulations</t>
+  </si>
+  <si>
+    <t>Lane Media: Simulations (FLRC Upstairs)</t>
   </si>
   <si>
     <t>LANE-SKKAT</t>
   </si>
   <si>
-    <t>Lane -- Ref: School Catalogs</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: School Catalogs</t>
+    <t>Lane Ref: School Catalogs</t>
+  </si>
+  <si>
+    <t>Lane Reference: School Catalogs</t>
   </si>
   <si>
     <t>LANE-SOFT</t>
   </si>
   <si>
-    <t>Lane -- Staff: Software</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Software Collection</t>
+    <t>Lane Staff: Software</t>
+  </si>
+  <si>
+    <t>Lane Staff: Software Collection</t>
   </si>
   <si>
     <t>LANE-SOMCC</t>
   </si>
   <si>
-    <t>Lane -- Lane Career Center</t>
-  </si>
-  <si>
-    <t>Lane -- Lane Career Center Collection</t>
+    <t>Lane Lane Career Center</t>
+  </si>
+  <si>
+    <t>Lane Lane Career Center Collection</t>
   </si>
   <si>
     <t>LANE-SPAV</t>
   </si>
   <si>
-    <t>Lane -- Spec: AV</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: AV: By appointment only.</t>
+    <t>Lane Spec: AV</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: AV: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SPEC</t>
   </si>
   <si>
-    <t>Lane -- Spec: LC Class</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: LC Classification: By appointment only.</t>
+    <t>Lane Spec: LC Class</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: LC Classification: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SPLCO</t>
   </si>
   <si>
-    <t>Lane -- Spec: LC Oversize</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: LC Class Oversize: By appointment only.</t>
+    <t>Lane Spec: LC Oversize</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: LC Class Oversize: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SPOLD</t>
   </si>
   <si>
-    <t>Lane -- Spec: Old Class</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Old Classification: By appointment only</t>
+    <t>Lane Spec: Old Class</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Old Classification: By appointment only</t>
   </si>
   <si>
     <t>LANE-SPOO1</t>
   </si>
   <si>
-    <t>Lane -- Spec: Old Class Oversize</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Old Class Oversize: By appointment only</t>
+    <t>Lane Spec: Old Class Oversize</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Old Class Oversize: By appointment only</t>
   </si>
   <si>
     <t>LANE-SPOO2</t>
   </si>
   <si>
-    <t>Lane -- Spec: Old Class O - Folio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane -- Special Collections:Old Class O-Folio: By appointment only. </t>
+    <t>Lane Spec: Old Class O - Folio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane Special Collections:Old Class O-Folio: By appointment only. </t>
   </si>
   <si>
     <t>LANE-SPOO3</t>
   </si>
   <si>
-    <t>Lane -- Spec: Old Class O - Flat</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Old Class O- Flat: By appointment only.</t>
+    <t>Lane Spec: Old Class O - Flat</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Old Class O- Flat: By appointment only.</t>
   </si>
   <si>
     <t>LANE-SREF</t>
   </si>
   <si>
-    <t>Lane -- Spec: Reference</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Reference: By appointment only.</t>
+    <t>Lane Spec: Reference</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Reference: By appointment only.</t>
   </si>
   <si>
     <t>LANE-STEAM</t>
   </si>
   <si>
-    <t>Lane -- Offsite: LC Class</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: LC Classification (Click on \"Request\" Link Above)</t>
+    <t>Lane Offsite: LC Class</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: LC Classification (Click on \"Request\" Link Above)</t>
   </si>
   <si>
     <t>LANE-STOR</t>
   </si>
   <si>
-    <t>Lane -- Offsi: OldClass 1851-1924</t>
-  </si>
-  <si>
-    <t>Lane -- OFFSITE: Old Class (1851-1924) Click on \"Request\" Link Above</t>
+    <t>Lane Offsi: OldClass 1851-1924</t>
+  </si>
+  <si>
+    <t>Lane OFFSITE: Old Class (1851-1924) Click on \"Request\" Link Above</t>
   </si>
   <si>
     <t>LANE-STRG</t>
   </si>
   <si>
-    <t>Lane -- Spec: Offsight Stroage</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Offsight Storage</t>
+    <t>Lane Spec: Offsight Stroage</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Offsight Storage</t>
   </si>
   <si>
     <t>LANE-SUL</t>
   </si>
   <si>
-    <t>Lane -- On Campus</t>
+    <t>Lane On Campus</t>
   </si>
   <si>
     <t>LANE-TELBK</t>
   </si>
   <si>
-    <t>Lane -- Ref: Telephone Books</t>
-  </si>
-  <si>
-    <t>Lane -- Reference: Telephone Books</t>
+    <t>Lane Ref: Telephone Books</t>
+  </si>
+  <si>
+    <t>Lane Reference: Telephone Books</t>
   </si>
   <si>
     <t>LANE-TEST</t>
   </si>
   <si>
-    <t>Lane -- Exam Questions</t>
-  </si>
-  <si>
-    <t>Lane -- Reserves: Examination Questions File</t>
+    <t>Lane Exam Questions</t>
+  </si>
+  <si>
+    <t>Lane Reserves: Examination Questions File</t>
   </si>
   <si>
     <t>LANE-THSS</t>
   </si>
   <si>
-    <t>Lane -- Books: Stanf Theses</t>
-  </si>
-  <si>
-    <t>Lane -- Books: Stanford Theses (Downstairs)</t>
+    <t>Lane Books: Stanf Theses</t>
+  </si>
+  <si>
+    <t>Lane Books: Stanford Theses (Downstairs)</t>
   </si>
   <si>
     <t>LANE-TS</t>
   </si>
   <si>
-    <t>Lane -- Staff: RM Coll</t>
-  </si>
-  <si>
-    <t>Lane -- Staff: Resource Management Collection</t>
+    <t>Lane Staff: RM Coll</t>
+  </si>
+  <si>
+    <t>Lane Staff: Resource Management Collection</t>
   </si>
   <si>
     <t>LANE-WKSTA</t>
   </si>
   <si>
-    <t>Lane -- Teaching Lab</t>
-  </si>
-  <si>
-    <t>Lane -- Teaching Lab (Alway M206)</t>
+    <t>Lane  Teaching Lab</t>
+  </si>
+  <si>
+    <t>Lane  Teaching Lab (Alway M206)</t>
   </si>
   <si>
     <t>LANE-WKSTB</t>
   </si>
   <si>
-    <t>Lane --  Workstations</t>
-  </si>
-  <si>
-    <t>Lane -- Workstations (1st Floor)</t>
+    <t>Lane   Workstations</t>
+  </si>
+  <si>
+    <t>Lane  Workstations (1st Floor)</t>
   </si>
   <si>
     <t>LANE-WKSTC</t>
   </si>
   <si>
-    <t>Lane --  Tech Studio</t>
-  </si>
-  <si>
-    <t>Lane -- Tech Studio</t>
+    <t>Lane   Tech Studio</t>
+  </si>
+  <si>
+    <t>Lane  Tech Studio</t>
   </si>
   <si>
     <t>LANE-WKSTD</t>
   </si>
   <si>
-    <t>Lane -- Spec: Display</t>
-  </si>
-  <si>
-    <t>Lane -- Special Collections: Display</t>
+    <t>Lane Spec: Display</t>
+  </si>
+  <si>
+    <t>Lane Special Collections: Display</t>
   </si>
   <si>
     <t>LANE-WKSTE</t>
   </si>
   <si>
-    <t>Lane -- Study Space</t>
-  </si>
-  <si>
-    <t>Lane -- Study Space (Alway M051)</t>
+    <t>Lane  Study Space</t>
+  </si>
+  <si>
+    <t>Lane  Study Space (Alway M051)</t>
   </si>
   <si>
     <t>select 'LANE-' || LOCATION_CODE AS code,
     CASE SUBSTR(LOCATION_NAME,0,5)
-        WHEN 'Lane:' THEN 'Lane --' || SUBSTR(LOCATION_NAME,6)
-        ELSE 'Lane -- ' || LOCATION_NAME
+        WHEN 'Lane:' THEN 'Lane ' || SUBSTR(LOCATION_NAME,6)
+        ELSE 'Lane ' || LOCATION_NAME
     END as name, 
     'TRUE' AS isActive, 
     '' as description,
     CASE SUBSTR(LOCATION_DISPLAY_NAME,0,5)
-        WHEN 'Lane:' THEN 'Lane --' || SUBSTR(replace(LOCATION_DISPLAY_NAME,'"','\"'),6)
-        ELSE 'Lane -- ' || replace(LOCATION_DISPLAY_NAME,'"','\"')
+        WHEN 'Lane:' THEN 'Lane ' || SUBSTR(replace(LOCATION_DISPLAY_NAME,'"','\"'),6)
+        ELSE 'Lane ' || replace(LOCATION_DISPLAY_NAME,'"','\"')
     END as discoveryDisplayName, 
     'SU' AS institutionCode,
     'MED' AS campusCode,
@@ -1658,11 +1658,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
“isActive” column needs to be in lowercase
</commit_message>
<xml_diff>
--- a/lane-locations.xlsx
+++ b/lane-locations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmax/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmax/Desktop/ILS-replacement/folio/repos/folio-lane-migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6383CC57-2C66-2443-A6AB-13275CF9F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21910829-5033-CC4C-B33F-136AB8640C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Lane  Acquisitions</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>true</t>
   </si>
   <si>
     <t>Lane ACQ</t>
@@ -1282,7 +1282,7 @@
         WHEN 'Lane:' THEN 'Lane ' || SUBSTR(LOCATION_NAME,6)
         ELSE 'Lane ' || LOCATION_NAME
     END as name, 
-    'TRUE' AS isActive, 
+    'true' AS isActive, 
     '' as description,
     CASE SUBSTR(LOCATION_DISPLAY_NAME,0,5)
         WHEN 'Lane:' THEN 'Lane ' || SUBSTR(replace(LOCATION_DISPLAY_NAME,'"','\"'),6)
@@ -1652,7 +1652,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>